<commit_message>
QR Code Scanner code w test file
</commit_message>
<xml_diff>
--- a/ActionDescriptionsShortened.xlsx
+++ b/ActionDescriptionsShortened.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Action name</t>
   </si>
@@ -43,15 +43,6 @@
     <t>No Contact</t>
   </si>
   <si>
-    <t>Index finger, pull towards</t>
-  </si>
-  <si>
-    <t>Index finger, push left</t>
-  </si>
-  <si>
-    <t>Index finger, push away</t>
-  </si>
-  <si>
     <t>Index finger, push right</t>
   </si>
   <si>
@@ -89,18 +80,6 @@
   </si>
   <si>
     <t>Pinch, thumb down</t>
-  </si>
-  <si>
-    <t>No contact</t>
-  </si>
-  <si>
-    <t>Pinch, thumb up</t>
-  </si>
-  <si>
-    <t>Draw word</t>
-  </si>
-  <si>
-    <t>Pinch-zoom</t>
   </si>
 </sst>
 </file>
@@ -170,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -198,9 +177,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -513,15 +489,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="13.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
@@ -579,7 +555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -598,34 +574,34 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6">
         <v>5</v>
@@ -634,9 +610,9 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="6">
         <v>5</v>
@@ -645,9 +621,9 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A12" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="6">
         <v>5</v>
@@ -658,43 +634,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6">
         <v>5</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>6</v>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>5</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>6</v>
@@ -702,73 +678,73 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6">
         <v>5</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="C18" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A20" s="5" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="38.25" customFormat="1" s="1">
+      <c r="A20" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="B20" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A21" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A22" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B22" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A23" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B23" s="6">
         <v>5</v>
@@ -777,147 +753,15 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="27.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A24" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B24" s="6">
         <v>5</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="38.25" customFormat="1" s="1">
-      <c r="A25" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="6">
-        <v>5</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="27.75" customFormat="1" s="1">
-      <c r="A26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="6">
-        <v>5</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="27.75" customFormat="1" s="1">
-      <c r="A27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="6">
-        <v>5</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="27.75" customFormat="1" s="1">
-      <c r="A28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="6">
-        <v>5</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A29" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="6">
-        <v>5</v>
-      </c>
-      <c r="C29" s="7" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A30" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="6">
-        <v>5</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="6">
-        <v>5</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="6">
-        <v>5</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="6">
-        <v>5</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="6">
-        <v>5</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A35" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="6">
-        <v>5</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A36" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="6">
-        <v>5</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file output details readme
</commit_message>
<xml_diff>
--- a/ActionDescriptionsShortened.xlsx
+++ b/ActionDescriptionsShortened.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>Action name</t>
   </si>
@@ -65,21 +65,6 @@
   </si>
   <si>
     <t>Fingertips down, pull towards</t>
-  </si>
-  <si>
-    <t>Grasp edge, thumb down, uncurled fingers</t>
-  </si>
-  <si>
-    <t>Grasp edge, thumb up, uncurled fingers</t>
-  </si>
-  <si>
-    <t>Grasp edge, thumb down, curled fingers</t>
-  </si>
-  <si>
-    <t>Grasp edge, thumb up, curled fingers</t>
-  </si>
-  <si>
-    <t>Pinch, thumb down</t>
   </si>
 </sst>
 </file>
@@ -149,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -173,9 +158,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -489,15 +471,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="13.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
@@ -709,61 +691,6 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="38.25" customFormat="1" s="1">
-      <c r="A20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="6">
-        <v>5</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="27.75" customFormat="1" s="1">
-      <c r="A21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="6">
-        <v>5</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="27.75" customFormat="1" s="1">
-      <c r="A22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="6">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="27.75" customFormat="1" s="1">
-      <c r="A23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="6">
-        <v>5</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="6">
-        <v>5</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>